<commit_message>
Schutz von Erfassungsdateien verstärkt
</commit_message>
<xml_diff>
--- a/templates/zeiterfassunsboegen.xlsx
+++ b/templates/zeiterfassunsboegen.xlsx
@@ -1,35 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\stephan\projects\wegpiraten\vorlagen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\stephan\projects\wegpiraten\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09516EA4-F229-4A52-9390-CA7BB045C345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D306882F-6B7E-4AA6-80EB-82EC68805361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="9r/TxM3zBcSjnJTI/hP9y4R5VkDU9X45pyxBQ1SRhdgGa0G4N9+kmOzqUscJS/8FfSdUOZhKQAU6CU1O1OaWPA==" workbookSaltValue="Ey8SgEponXL1upYzdwO0ww==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-2385" windowWidth="38640" windowHeight="21120" tabRatio="709" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="709" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitszeiterfassung" sheetId="47" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_13._ML">#REF!</definedName>
-    <definedName name="_BVG1">#REF!</definedName>
-    <definedName name="_BVG2">#REF!</definedName>
-    <definedName name="_BVG3">#REF!</definedName>
-    <definedName name="AHV">#REF!</definedName>
-    <definedName name="ALV">#REF!</definedName>
-    <definedName name="KiZu1">#REF!</definedName>
-    <definedName name="KiZu2">#REF!</definedName>
-    <definedName name="KTG">#REF!</definedName>
-    <definedName name="NBU">#REF!</definedName>
-    <definedName name="Vollzug">#REF!</definedName>
-    <definedName name="VRM">#REF!</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -46,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Monat/Jahr:</t>
   </si>
@@ -105,9 +91,6 @@
     <t>Klient-Nr.:</t>
   </si>
   <si>
-    <t>V5.0 autom</t>
-  </si>
-  <si>
     <t>km</t>
   </si>
   <si>
@@ -123,7 +106,7 @@
     <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
     <numFmt numFmtId="166" formatCode="[$-407]mmmm\ yy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -216,6 +199,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -449,164 +447,164 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="17" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="17" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -615,26 +613,6 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -646,458 +624,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
+        <sz val="11"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1105,75 +636,8 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1224,6 +688,532 @@
           <color indexed="64"/>
         </bottom>
       </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00;\-0.00;;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -1328,15 +1318,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2923342</xdr:colOff>
+      <xdr:colOff>2904292</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>4753352</xdr:colOff>
+      <xdr:colOff>4734302</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>36692</xdr:rowOff>
+      <xdr:rowOff>74792</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1365,8 +1355,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7923967" y="0"/>
-          <a:ext cx="1830010" cy="1522592"/>
+          <a:off x="7914442" y="38100"/>
+          <a:ext cx="1830010" cy="1547992"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1379,21 +1369,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B2FD7CF-661B-4404-A2DA-55AA5D212FF4}" name="Tabelle1" displayName="Tabelle1" ref="A10:H29" totalsRowCount="1" headerRowDxfId="17" dataDxfId="15" totalsRowDxfId="16" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B2FD7CF-661B-4404-A2DA-55AA5D212FF4}" name="Tabelle1" displayName="Tabelle1" ref="A10:H29" totalsRowCount="1" headerRowDxfId="0" dataDxfId="2" totalsRowDxfId="18" tableBorderDxfId="19">
   <autoFilter ref="A10:H28" xr:uid="{3B2FD7CF-661B-4404-A2DA-55AA5D212FF4}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5EAB673B-37E4-4253-B726-3AE18B468C44}" name="Uhrzeit" dataDxfId="14" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{EDDDF320-FF16-41E3-BAD3-C9289AAC0914}" name="Datum" totalsRowLabel="Insgesamt" dataDxfId="13" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{97372A55-45C0-42B9-9E1A-EB9E4C2413D0}" name="Fahrtzeit" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{91B4AA5C-70E3-484A-B8D3-5B26B30981A9}" name="km" totalsRowFunction="min" dataDxfId="11" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{ABA3D436-0B90-49E6-A8BA-55DD855D507E}" name="Direkter Fallkontakt" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{9BE51089-74AE-4C2E-A355-650C3C094E09}" name="Indirekte Fallbearbeitung" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{6D56DF91-8B1E-44E1-A0F2-D5546E2E6E03}" name="Stunden" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="1">
+    <tableColumn id="1" xr3:uid="{5EAB673B-37E4-4253-B726-3AE18B468C44}" name="Uhrzeit" dataDxfId="9" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{EDDDF320-FF16-41E3-BAD3-C9289AAC0914}" name="Datum" totalsRowLabel="Insgesamt" dataDxfId="8" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{97372A55-45C0-42B9-9E1A-EB9E4C2413D0}" name="Fahrtzeit" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{91B4AA5C-70E3-484A-B8D3-5B26B30981A9}" name="km" totalsRowFunction="min" dataDxfId="6" totalsRowDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{ABA3D436-0B90-49E6-A8BA-55DD855D507E}" name="Direkter Fallkontakt" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{9BE51089-74AE-4C2E-A355-650C3C094E09}" name="Indirekte Fallbearbeitung" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{6D56DF91-8B1E-44E1-A0F2-D5546E2E6E03}" name="Stunden" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="11">
       <calculatedColumnFormula>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{006ED2E5-4DD9-4CD7-98C5-B09999D81256}" name="Notizen           " dataDxfId="8" totalsRowDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{006ED2E5-4DD9-4CD7-98C5-B09999D81256}" name="Notizen           " dataDxfId="3" totalsRowDxfId="10"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1747,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3B06A5-8E9D-470B-9030-AC4032ABA6C5}">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A3:H103"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1766,11 +1756,6 @@
     <col min="9" max="16384" width="11.26953125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="3" spans="1:8" ht="22" x14ac:dyDescent="0.5">
       <c r="A3" s="16" t="s">
         <v>14</v>
@@ -1780,98 +1765,98 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21" t="s">
+      <c r="B5" s="56"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="22"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="28"/>
+      <c r="A6" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="58"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="28"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="24"/>
     </row>
     <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28" t="s">
+      <c r="B8" s="58"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="24"/>
     </row>
     <row r="9" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="34"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="29"/>
     </row>
     <row r="10" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="36" t="s">
+      <c r="D10" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="H10" s="64" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="67"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="40">
+      <c r="G11" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
@@ -1884,7 +1869,7 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="40">
+      <c r="G12" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
@@ -1897,7 +1882,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="40">
+      <c r="G13" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
@@ -1910,7 +1895,7 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="40">
+      <c r="G14" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
@@ -1923,264 +1908,264 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="40">
+      <c r="G15" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:8" s="41" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" s="31" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="40">
+      <c r="G16" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="40">
+      <c r="G17" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="40">
+      <c r="G18" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="40">
+      <c r="G19" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="40">
+      <c r="G20" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="40">
+      <c r="G21" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="40">
+      <c r="G22" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="40">
+      <c r="G23" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="40">
+      <c r="G24" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="40">
+      <c r="G25" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="40">
+      <c r="G26" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="40">
+      <c r="G27" s="62">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8" s="42" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" s="32" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="43">
+      <c r="G28" s="63">
         <f>SUM(Tabelle1[[#This Row],[Fahrtzeit]],Tabelle1[[#This Row],[Direkter Fallkontakt]],Tabelle1[[#This Row],[Indirekte Fallbearbeitung]])</f>
         <v>0</v>
       </c>
       <c r="H28" s="9"/>
     </row>
-    <row r="29" spans="1:8" s="42" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="44"/>
-      <c r="B29" s="45" t="s">
+    <row r="29" spans="1:8" s="32" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="33"/>
+      <c r="B29" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="46">
+      <c r="C29" s="35">
         <f>SUBTOTAL(109,Tabelle1[Fahrtzeit])</f>
         <v>0</v>
       </c>
-      <c r="D29" s="46">
+      <c r="D29" s="35">
         <f>SUBTOTAL(105,Tabelle1[km])</f>
         <v>0</v>
       </c>
-      <c r="E29" s="46">
+      <c r="E29" s="35">
         <f>SUBTOTAL(109,Tabelle1[Direkter Fallkontakt])</f>
         <v>0</v>
       </c>
-      <c r="F29" s="46">
+      <c r="F29" s="35">
         <f>SUBTOTAL(109,Tabelle1[Indirekte Fallbearbeitung])</f>
         <v>0</v>
       </c>
-      <c r="G29" s="47">
+      <c r="G29" s="36">
         <f>SUBTOTAL(109,Tabelle1[Stunden])</f>
         <v>0</v>
       </c>
-      <c r="H29" s="48"/>
-    </row>
-    <row r="30" spans="1:8" s="42" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="49"/>
+      <c r="H29" s="37"/>
+    </row>
+    <row r="30" spans="1:8" s="32" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="38"/>
       <c r="B30" s="11"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="51"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="40"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:8" s="42" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="52" t="s">
+    <row r="31" spans="1:8" s="32" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="53"/>
-      <c r="C31" s="54" t="s">
+      <c r="B31" s="61"/>
+      <c r="C31" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="57" t="s">
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="58"/>
-    </row>
-    <row r="32" spans="1:8" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="59">
+      <c r="H31" s="54"/>
+    </row>
+    <row r="32" spans="1:8" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="42">
         <f>C7</f>
         <v>0</v>
       </c>
-      <c r="B32" s="60"/>
-      <c r="C32" s="59">
+      <c r="B32" s="43"/>
+      <c r="C32" s="42">
         <f>Tabelle1[[#Totals],[Stunden]]</f>
         <v>0</v>
       </c>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="59">
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="42">
         <f>C32-A32</f>
         <v>0</v>
       </c>
-      <c r="H32" s="61"/>
-    </row>
-    <row r="33" spans="1:8" s="42" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="63"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="65"/>
-    </row>
-    <row r="34" spans="1:8" s="42" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H32" s="49"/>
+    </row>
+    <row r="33" spans="1:8" s="32" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="44"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="51"/>
+    </row>
+    <row r="34" spans="1:8" s="32" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -2190,7 +2175,7 @@
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" s="42" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" s="32" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -2242,18 +2227,18 @@
     </row>
     <row r="103" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KucHu47xtR3s/aCCSBMFfeZY4r9mrSSXuNpOtxyNng+zfehVq9OBYT3cGfLPYhQapCUlBkA856JnyQWtpHQUSQ==" saltValue="OrXmpXkTaZl2xNzJpFGjTA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="N3Ewu0rrFmXuBreMUn+KGt6i77oo/3HbDmwUXtTXzAv/8smMs2HhDiHyxjPGHl/eyU/I6YTz9sfnRN7Xe//rfg==" saltValue="sE9klEljYbRF2jDgybgKkA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="10">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="C31:F31"/>
     <mergeCell ref="C32:F33"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="G32:H33"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2265,6 +2250,8 @@
  www.wegpiraten.ch&amp;R&amp;9Sozialpädagogische
 Familienbegleitung&amp;K00+000A&amp;K000000
 </oddFooter>
+    <firstHeader>&amp;LV5.0 autom
+&amp;RC3 - Vertraulich</firstHeader>
     <firstFooter xml:space="preserve">&amp;L&amp;7Wegpiraten GmbH
 Alpenstrasse 2
 3800 Interlaken&amp;C&amp;7Tel: 076 790 67 56

</xml_diff>